<commit_message>
Add a small note to identify ovens
</commit_message>
<xml_diff>
--- a/docs/example_schedule.xlsx
+++ b/docs/example_schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xfer_self\waittime\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cel\projects\waittime\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C022031-4D0E-4E9F-A3EB-524E66DE350E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9F9DA05-5520-4639-88E7-D8A16C3199FA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-60" windowWidth="29040" windowHeight="15840" xr2:uid="{D4D6C81B-4C99-4285-9FAA-35BED5DD3C4C}"/>
+    <workbookView xWindow="11055" yWindow="3120" windowWidth="38700" windowHeight="15375" xr2:uid="{D4D6C81B-4C99-4285-9FAA-35BED5DD3C4C}"/>
   </bookViews>
   <sheets>
     <sheet name="1-25-21" sheetId="7" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="37">
   <si>
     <t>MON</t>
   </si>
@@ -137,6 +137,9 @@
   </si>
   <si>
     <t>Delays</t>
+  </si>
+  <si>
+    <t>&lt; - ovens</t>
   </si>
 </sst>
 </file>
@@ -1229,7 +1232,7 @@
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="T14" sqref="T14"/>
+      <selection pane="bottomLeft" activeCell="Q2" sqref="Q2:Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1288,7 +1291,9 @@
         <v>15</v>
       </c>
       <c r="N1" s="67"/>
-      <c r="P1" s="41"/>
+      <c r="P1" s="2" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="2" spans="1:27" ht="18.75" x14ac:dyDescent="0.35">
       <c r="A2" s="41" t="s">

</xml_diff>